<commit_message>
Updated case-control tables with duration
</commit_message>
<xml_diff>
--- a/Supplementary_Material/Outputs/CC_T2D_table.xlsx
+++ b/Supplementary_Material/Outputs/CC_T2D_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -689,6 +689,33 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4 [1,15]</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0 (0%)</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>10 [5,20]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>0 (0%)</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>